<commit_message>
Added print function, few conversion functions and empty function finder
</commit_message>
<xml_diff>
--- a/input_files/data_table.xlsx
+++ b/input_files/data_table.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Id</t>
   </si>
@@ -68,6 +68,27 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
   </si>
 </sst>
 </file>
@@ -76,7 +97,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;$&quot;_ ;_ * \(#,##0.00\)\ &quot;$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;$&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;$&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;$&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -132,13 +153,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -425,9 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -553,10 +572,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,6 +595,33 @@
       <c r="A2" t="s">
         <v>13</v>
       </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -584,14 +630,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:B9"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="7.35" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="7.35" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added mapping for columns, functional with input checking
</commit_message>
<xml_diff>
--- a/input_files/data_table.xlsx
+++ b/input_files/data_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -574,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +635,7 @@
   <dimension ref="B3:B9"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added mapping functionality, possiblity to add multiple cells to a same column + updated functions in tools and parsing function
</commit_message>
<xml_diff>
--- a/input_files/data_table.xlsx
+++ b/input_files/data_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Id</t>
   </si>
@@ -89,6 +89,15 @@
   </si>
   <si>
     <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
   </si>
 </sst>
 </file>
@@ -446,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -574,10 +583,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,6 +632,30 @@
       </c>
       <c r="B5" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Possibility to generate excel files individually with column mapping!
</commit_message>
<xml_diff>
--- a/input_files/data_table.xlsx
+++ b/input_files/data_table.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Id</t>
   </si>
@@ -88,16 +88,7 @@
     <t>C7</t>
   </si>
   <si>
-    <t>C8</t>
-  </si>
-  <si>
     <t>C9</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>C11</t>
   </si>
 </sst>
 </file>
@@ -108,7 +99,7 @@
     <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;$&quot;_ ;_ * \(#,##0.00\)\ &quot;$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;$&quot;_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;$&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +122,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -140,12 +139,51 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -154,7 +192,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -171,6 +209,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -456,7 +498,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,10 +625,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,30 +676,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -665,10 +683,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B9"/>
+  <dimension ref="B3:E9"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,28 +696,45 @@
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="2:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:2" ht="7.35" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="2:5" ht="7.35" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="2:2" ht="7.35" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="2:5" ht="7.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
         <v>4</v>
       </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New class structure, changes still need to be made in the future (additonal classes to add and remove certain files)
</commit_message>
<xml_diff>
--- a/input_files/data_table.xlsx
+++ b/input_files/data_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -49,18 +49,12 @@
     <t>32 Brook St, Washington, DC</t>
   </si>
   <si>
-    <t>robert.lee@gmail.com</t>
-  </si>
-  <si>
     <t>Ann Froster</t>
   </si>
   <si>
     <t>1422 Jay St, Seattle, WA</t>
   </si>
   <si>
-    <t>a.froster@yahoo.com</t>
-  </si>
-  <si>
     <t>Column</t>
   </si>
   <si>
@@ -73,9 +67,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -89,6 +80,15 @@
   </si>
   <si>
     <t>C9</t>
+  </si>
+  <si>
+    <t>lesroutes2005@yahoo.fr</t>
+  </si>
+  <si>
+    <t>lesroute2014@gmail.com</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -497,15 +497,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
@@ -537,7 +537,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E2" s="5">
         <v>350</v>
@@ -548,13 +548,13 @@
         <v>253665</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E3" s="4">
         <v>36</v>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,42 +638,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality for sending static and dynamic emails (content can be adapted depending on what is needed)
</commit_message>
<xml_diff>
--- a/input_files/data_table.xlsx
+++ b/input_files/data_table.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="mapping" sheetId="2" r:id="rId2"/>
-    <sheet name="template" sheetId="3" r:id="rId3"/>
+    <sheet name="mail" sheetId="4" r:id="rId3"/>
+    <sheet name="template" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Id</t>
   </si>
@@ -85,10 +86,28 @@
     <t>lesroutes2005@yahoo.fr</t>
   </si>
   <si>
-    <t>lesroute2014@gmail.com</t>
-  </si>
-  <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>This is a test</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Recipient</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>lesroutes2014@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -192,7 +211,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -213,6 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -230,6 +250,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>403005</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4733926" y="447676"/>
+          <a:ext cx="917354" cy="838199"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +634,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E3" s="4">
         <v>36</v>
@@ -627,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,10 +717,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -662,7 +742,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -674,6 +754,59 @@
       </c>
       <c r="B5" t="s">
         <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -681,12 +814,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E9"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,5 +872,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>